<commit_message>
Upload source code from zip to branch HuyHoang
</commit_message>
<xml_diff>
--- a/employee.xlsx
+++ b/employee.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -68,90 +68,102 @@
     <t>11-04-2003</t>
   </si>
   <si>
-    <t>Admin2</t>
+    <t>Nhân viên quản lý kho</t>
   </si>
   <si>
     <t>2.000.000</t>
   </si>
   <si>
+    <t>Trần Văn</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>15-01-1990</t>
+  </si>
+  <si>
+    <t>3.000.000</t>
+  </si>
+  <si>
+    <t>7.500.000</t>
+  </si>
+  <si>
+    <t>Lê Thị</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>20-02-1988</t>
+  </si>
+  <si>
+    <t>3.500.000</t>
+  </si>
+  <si>
+    <t>8.750.000</t>
+  </si>
+  <si>
+    <t>Phạm Minh</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>25-03-1985</t>
+  </si>
+  <si>
     <t>4.000.000</t>
   </si>
   <si>
-    <t>Trần Văn</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>15-01-1990</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>3.000.000</t>
-  </si>
-  <si>
-    <t>Lê Thị</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>20-02-1988</t>
-  </si>
-  <si>
-    <t>3.500.000</t>
-  </si>
-  <si>
-    <t>Phạm Minh</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>25-03-1985</t>
+    <t>10.000.000</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>30-04-1992</t>
+  </si>
+  <si>
+    <t>4.500.000</t>
+  </si>
+  <si>
+    <t>11.250.000</t>
+  </si>
+  <si>
+    <t>Đỗ Văn</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>05-05-1995</t>
+  </si>
+  <si>
+    <t>2.800.000</t>
+  </si>
+  <si>
+    <t>7.000.000</t>
+  </si>
+  <si>
+    <t>Bùi Thị</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>10-06-1993</t>
+  </si>
+  <si>
+    <t>3.200.000</t>
   </si>
   <si>
     <t>8.000.000</t>
   </si>
   <si>
-    <t>Nguyễn Thị</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>30-04-1992</t>
-  </si>
-  <si>
-    <t>4.500.000</t>
-  </si>
-  <si>
-    <t>Đỗ Văn</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>05-05-1995</t>
-  </si>
-  <si>
-    <t>2.800.000</t>
-  </si>
-  <si>
-    <t>Bùi Thị</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>10-06-1993</t>
-  </si>
-  <si>
-    <t>3.200.000</t>
-  </si>
-  <si>
     <t>Ngô Minh</t>
   </si>
   <si>
@@ -164,6 +176,9 @@
     <t>2.900.000</t>
   </si>
   <si>
+    <t>7.250.000</t>
+  </si>
+  <si>
     <t>Trịnh Văn</t>
   </si>
   <si>
@@ -176,6 +191,9 @@
     <t>3.100.000</t>
   </si>
   <si>
+    <t>7.750.000</t>
+  </si>
+  <si>
     <t>Ngưng hoat động</t>
   </si>
   <si>
@@ -204,18 +222,6 @@
   </si>
   <si>
     <t>12.950.000</t>
-  </si>
-  <si>
-    <t>Pro vip</t>
-  </si>
-  <si>
-    <t>ALo</t>
-  </si>
-  <si>
-    <t>2.999.999</t>
-  </si>
-  <si>
-    <t>10.499.996,5</t>
   </si>
 </sst>
 </file>
@@ -260,7 +266,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -270,9 +276,9 @@
     <col min="2" max="2" width="13.984375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.4375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.76171875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="10.81640625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="20.8984375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="9.953125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="12.734375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="11.15234375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="16.67578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -348,7 +354,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s" s="0">
         <v>14</v>
@@ -359,22 +365,22 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="D4" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="E4" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="G4" t="s" s="0">
         <v>24</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>25</v>
       </c>
       <c r="H4" t="s" s="0">
         <v>14</v>
@@ -385,19 +391,19 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="D5" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="E5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s" s="0">
         <v>28</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>29</v>
       </c>
       <c r="G5" t="s" s="0">
         <v>29</v>
@@ -423,10 +429,10 @@
         <v>18</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s" s="0">
         <v>14</v>
@@ -437,22 +443,22 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H7" t="s" s="0">
         <v>14</v>
@@ -463,22 +469,22 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H8" t="s" s="0">
         <v>14</v>
@@ -489,22 +495,22 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s" s="0">
         <v>14</v>
@@ -515,22 +521,22 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H10" t="s" s="0">
         <v>14</v>
@@ -541,25 +547,25 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="H11" t="s" s="0">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
@@ -567,22 +573,22 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s" s="0">
         <v>11</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" t="s" s="0">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="H12" t="s" s="0">
         <v>14</v>
@@ -593,50 +599,24 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s" s="0">
         <v>11</v>
       </c>
       <c r="F13" t="s" s="0">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="G13" t="s" s="0">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="H13" t="s" s="0">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n" s="0">
-        <v>13.0</v>
-      </c>
-      <c r="B14" t="s" s="0">
-        <v>64</v>
-      </c>
-      <c r="C14" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="D14" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="E14" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s" s="0">
-        <v>66</v>
-      </c>
-      <c r="G14" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="H14" t="s" s="0">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Chuan bi cham do an
</commit_message>
<xml_diff>
--- a/employee.xlsx
+++ b/employee.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -74,19 +74,22 @@
     <t>2.000.000</t>
   </si>
   <si>
-    <t>Trần Văn</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>15-01-1990</t>
+    <t>Tần Thiên</t>
+  </si>
+  <si>
+    <t>Lang</t>
+  </si>
+  <si>
+    <t>15-01-2000</t>
+  </si>
+  <si>
+    <t>Nhân viên bán hàng</t>
   </si>
   <si>
     <t>3.000.000</t>
   </si>
   <si>
-    <t>7.500.000</t>
+    <t>6.000.000</t>
   </si>
   <si>
     <t>Lê Thị</t>
@@ -101,7 +104,7 @@
     <t>3.500.000</t>
   </si>
   <si>
-    <t>8.750.000</t>
+    <t>7.000.000</t>
   </si>
   <si>
     <t>Phạm Minh</t>
@@ -116,7 +119,7 @@
     <t>4.000.000</t>
   </si>
   <si>
-    <t>10.000.000</t>
+    <t>8.000.000</t>
   </si>
   <si>
     <t>Nguyễn Thị</t>
@@ -131,7 +134,7 @@
     <t>4.500.000</t>
   </si>
   <si>
-    <t>11.250.000</t>
+    <t>9.000.000</t>
   </si>
   <si>
     <t>Đỗ Văn</t>
@@ -143,10 +146,13 @@
     <t>05-05-1995</t>
   </si>
   <si>
+    <t>Quản lý chức vụ</t>
+  </si>
+  <si>
     <t>2.800.000</t>
   </si>
   <si>
-    <t>7.000.000</t>
+    <t>7.840.000</t>
   </si>
   <si>
     <t>Bùi Thị</t>
@@ -158,10 +164,13 @@
     <t>10-06-1993</t>
   </si>
   <si>
+    <t>Quản lý cửa hàng</t>
+  </si>
+  <si>
     <t>3.200.000</t>
   </si>
   <si>
-    <t>8.000.000</t>
+    <t>8.320.000</t>
   </si>
   <si>
     <t>Ngô Minh</t>
@@ -173,10 +182,13 @@
     <t>15-07-1991</t>
   </si>
   <si>
+    <t>Nhân viên chăm sóc khách hàng</t>
+  </si>
+  <si>
     <t>2.900.000</t>
   </si>
   <si>
-    <t>7.250.000</t>
+    <t>6.380.000</t>
   </si>
   <si>
     <t>Trịnh Văn</t>
@@ -276,7 +288,7 @@
     <col min="2" max="2" width="13.984375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.4375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.76171875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="20.8984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="29.60546875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="9.953125" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="11.15234375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="16.67578125" customWidth="true" bestFit="true"/>
@@ -374,13 +386,13 @@
         <v>22</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s" s="0">
         <v>14</v>
@@ -391,22 +403,22 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H5" t="s" s="0">
         <v>14</v>
@@ -417,22 +429,22 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H6" t="s" s="0">
         <v>14</v>
@@ -443,22 +455,22 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H7" t="s" s="0">
         <v>14</v>
@@ -469,22 +481,22 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H8" t="s" s="0">
         <v>14</v>
@@ -495,22 +507,22 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H9" t="s" s="0">
         <v>14</v>
@@ -521,22 +533,22 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H10" t="s" s="0">
         <v>14</v>
@@ -547,25 +559,25 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s" s="0">
         <v>18</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H11" t="s" s="0">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12">
@@ -573,22 +585,22 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E12" t="s" s="0">
         <v>11</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G12" t="s" s="0">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="H12" t="s" s="0">
         <v>14</v>
@@ -599,25 +611,25 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s" s="0">
         <v>11</v>
       </c>
       <c r="F13" t="s" s="0">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G13" t="s" s="0">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H13" t="s" s="0">
-        <v>60</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>